<commit_message>
update centrality actors analysis
</commit_message>
<xml_diff>
--- a/A14/Redes Sociales/MedidasRedesPracticaParteI-1.xlsx
+++ b/A14/Redes Sociales/MedidasRedesPracticaParteI-1.xlsx
@@ -1,28 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23720"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{439B0526-0E03-4318-BF4F-7FBE76273A5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="11715" windowHeight="3150"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="11715" windowHeight="3150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
-  <si>
-    <t xml:space="preserve">Nombre y apellidos del alumno: </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Laura Rodríguez Navas</t>
   </si>
   <si>
     <t>Medida</t>
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Número de nodos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Número de enlaces </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L</t>
+    </r>
   </si>
   <si>
     <r>
@@ -54,7 +107,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Número de enlaces </t>
+      <t xml:space="preserve">Densidad del grafo </t>
     </r>
     <r>
       <rPr>
@@ -65,12 +118,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>L</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Número de nodos </t>
+      <t>L/Lmax</t>
+    </r>
+  </si>
+  <si>
+    <t>0.004</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Grado medio </t>
     </r>
     <r>
       <rPr>
@@ -81,32 +137,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Distancia media </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>d</t>
+      <t>&lt;k&gt;</t>
     </r>
   </si>
   <si>
@@ -139,7 +170,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Grado medio </t>
+      <t xml:space="preserve">Distancia media </t>
     </r>
     <r>
       <rPr>
@@ -150,23 +181,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;k&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Densidad del grafo </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>L/Lmax</t>
+      <t>d</t>
     </r>
   </si>
   <si>
@@ -186,41 +201,23 @@
     </r>
   </si>
   <si>
-    <t>&lt;Añadir aquí el gráfico de la distribución de grados&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Añadir aquí el gráfico de la distribución de distancias&gt;</t>
+    <t>0.819</t>
   </si>
   <si>
     <t>Número de componentes conexas</t>
   </si>
   <si>
-    <t>XXX</t>
-  </si>
-  <si>
-    <t>XXX.XXX</t>
-  </si>
-  <si>
-    <t>X.XXX</t>
-  </si>
-  <si>
-    <t>Nota: En Gephi, este gráfico corresponde al de la medida de centralidad de distancia no normalizada</t>
-  </si>
-  <si>
     <t>Número de nodos componente gigante</t>
   </si>
   <si>
-    <t>% de aristas componente gigante</t>
-  </si>
-  <si>
-    <t>0.XXX</t>
+    <t>Número de aristas componente gigante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -322,10 +319,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -341,19 +338,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -372,21 +356,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -394,30 +363,43 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -426,29 +408,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,12 +454,111 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imatge 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CF410BC-6A81-4554-BFD6-6A55B8536750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="3429000"/>
+          <a:ext cx="5715000" cy="3810000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imatge 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADF9760-897F-40D4-BE77-65416FB6EC1B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4CF410BC-6A81-4554-BFD6-6A55B8536750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28575" y="7353300"/>
+          <a:ext cx="5715000" cy="3810000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -506,7 +600,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,9 +633,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,6 +685,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -749,20 +877,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.75" customWidth="1"/>
-    <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -770,7 +898,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +908,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -788,7 +916,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -796,11 +924,11 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
@@ -808,223 +936,209 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>14</v>
+    <row r="6" spans="1:6" ht="15.75">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1419</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" ht="15.75">
+      <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>14</v>
+      <c r="B7" s="7">
+        <v>3926</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>14</v>
+    <row r="8" spans="1:6" ht="15.75">
+      <c r="A8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1006071</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>16</v>
+    <row r="9" spans="1:6" ht="15.75">
+      <c r="A9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" ht="15.75">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>15</v>
+      <c r="B10" s="9">
+        <v>5533</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>14</v>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>15</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>15</v>
+    <row r="12" spans="1:6" ht="15.75">
+      <c r="A12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10">
+        <v>6783</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>16</v>
+    <row r="13" spans="1:6" ht="15.75">
+      <c r="A13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:6" ht="15.75">
+      <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>14</v>
+      <c r="B14" s="6">
+        <v>1</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:6" ht="15.75">
+      <c r="A15" s="13" t="s">
         <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1419</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="7">
+        <v>3926</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>14</v>
-      </c>
+    <row r="17" spans="1:6" ht="15.75">
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>20</v>
-      </c>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75">
+      <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+    <row r="23" spans="1:6" ht="15.75">
+      <c r="A23" s="5"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>12</v>
-      </c>
+    <row r="24" spans="1:6" ht="15.75">
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>17</v>
-      </c>
+    <row r="25" spans="1:6" ht="15.75">
+      <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1032,7 +1146,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1040,7 +1154,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1048,24 +1162,9 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>